<commit_message>
Add tests for task addition feature.
- add necessary docs
- fix issue with task constructor discovered during testing
</commit_message>
<xml_diff>
--- a/Docs/Lab02/Lab02_BBT_TCs_Form.xlsx
+++ b/Docs/Lab02/Lab02_BBT_TCs_Form.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11207"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28526"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{92E18F35-726E-CA4C-8C42-47DD506855A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96B0278C-6B03-4318-BE5C-433F831244D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20" yWindow="760" windowWidth="30240" windowHeight="17400" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="0" windowWidth="26010" windowHeight="20985" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Statement" sheetId="1" r:id="rId1"/>
@@ -146,7 +146,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="138">
   <si>
     <t>VVSS, Info Romana, 2024-2025</t>
   </si>
@@ -433,9 +433,6 @@
     <t>TC3_ECP</t>
   </si>
   <si>
-    <t>TC5_ECP</t>
-  </si>
-  <si>
     <t>Statistics</t>
   </si>
   <si>
@@ -491,9 +488,6 @@
   </si>
   <si>
     <t>Re-tested</t>
-  </si>
-  <si>
-    <t>not yet</t>
   </si>
   <si>
     <t>Copas Codrut -George</t>
@@ -546,9 +540,6 @@
   </si>
   <si>
     <t>end &lt; 1970-01-01</t>
-  </si>
-  <si>
-    <t>octav gay</t>
   </si>
   <si>
     <t>start</t>
@@ -742,18 +733,9 @@
     <t>"T8"</t>
   </si>
   <si>
-    <t>TC4-ECP</t>
-  </si>
-  <si>
-    <t>TC6_BVA</t>
-  </si>
-  <si>
     <t>TC7_BVA</t>
   </si>
   <si>
-    <t>TC8_BVA</t>
-  </si>
-  <si>
     <t>TC10_BVA</t>
   </si>
   <si>
@@ -767,13 +749,40 @@
   </si>
   <si>
     <t>TC13_BVA</t>
+  </si>
+  <si>
+    <t>EcpInvalidTestCase</t>
+  </si>
+  <si>
+    <t>EcpValidTestCase</t>
+  </si>
+  <si>
+    <t>TC2-ECP</t>
+  </si>
+  <si>
+    <t>"TestTask"</t>
+  </si>
+  <si>
+    <t>" Title"</t>
+  </si>
+  <si>
+    <t>BvaValidTestCase</t>
+  </si>
+  <si>
+    <t>BvaInvalidTestCase</t>
+  </si>
+  <si>
+    <t>done</t>
+  </si>
+  <si>
+    <t>done/not needed</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="30" x14ac:knownFonts="1">
+  <fonts count="30">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1415,7 +1424,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="120">
+  <cellXfs count="125">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -1516,210 +1525,6 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1727,8 +1532,223 @@
     <xf numFmtId="14" fontId="12" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1745,6 +1765,55 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>302173</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>72259</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>34</xdr:col>
+      <xdr:colOff>556272</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>57190</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AFE6FAB8-DA5D-0F9F-9313-E4F43DDCF3EF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12073759" y="3534104"/>
+          <a:ext cx="13260651" cy="2638793"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2040,39 +2109,39 @@
   <dimension ref="A1:O26"/>
   <sheetViews>
     <sheetView zoomScale="138" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="4" max="4" width="22.5" customWidth="1"/>
-    <col min="9" max="9" width="32.83203125" customWidth="1"/>
-    <col min="10" max="10" width="10.5" customWidth="1"/>
-    <col min="12" max="12" width="12.1640625" customWidth="1"/>
+    <col min="4" max="4" width="22.42578125" customWidth="1"/>
+    <col min="9" max="9" width="32.85546875" customWidth="1"/>
+    <col min="10" max="10" width="10.42578125" customWidth="1"/>
+    <col min="12" max="12" width="12.140625" customWidth="1"/>
     <col min="14" max="14" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="C1" s="45" t="s">
+    <row r="1" spans="2:10">
+      <c r="C1" s="53" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="46"/>
-      <c r="E1" s="46"/>
-      <c r="F1" s="47"/>
+      <c r="D1" s="54"/>
+      <c r="E1" s="54"/>
+      <c r="F1" s="55"/>
       <c r="H1" s="43" t="s">
         <v>1</v>
       </c>
       <c r="I1" s="43"/>
       <c r="J1" s="43"/>
     </row>
-    <row r="2" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="H2" s="48" t="s">
+    <row r="2" spans="2:10">
+      <c r="H2" s="56" t="s">
         <v>2</v>
       </c>
-      <c r="I2" s="48"/>
-      <c r="J2" s="48"/>
-    </row>
-    <row r="3" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="I2" s="56"/>
+      <c r="J2" s="56"/>
+    </row>
+    <row r="3" spans="2:10">
       <c r="H3" s="2"/>
       <c r="I3" s="2" t="s">
         <v>3</v>
@@ -2081,74 +2150,74 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:10">
       <c r="H4" s="2" t="s">
         <v>5</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="J4" s="2">
         <v>232</v>
       </c>
     </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:10">
       <c r="H5" s="2" t="s">
         <v>6</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="J5" s="2">
         <v>232</v>
       </c>
     </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:10">
       <c r="B6" s="29"/>
       <c r="H6" s="2" t="s">
         <v>7</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="J6" s="2">
         <v>232</v>
       </c>
     </row>
-    <row r="7" spans="2:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:10" ht="14.45" customHeight="1"/>
+    <row r="8" spans="2:10">
       <c r="B8" s="41" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:10">
       <c r="B9" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:10">
       <c r="B10" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:10">
       <c r="B11" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:10">
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
     </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:10">
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
     </row>
-    <row r="14" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:10">
       <c r="B14" t="s">
         <v>12</v>
       </c>
@@ -2156,7 +2225,7 @@
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
     </row>
-    <row r="15" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:10">
       <c r="B15" t="s">
         <v>13</v>
       </c>
@@ -2164,7 +2233,7 @@
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
     </row>
-    <row r="16" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:10">
       <c r="B16" t="s">
         <v>14</v>
       </c>
@@ -2172,32 +2241,32 @@
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:15">
       <c r="B17" s="1"/>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:15">
       <c r="B18" s="41" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:15">
       <c r="B19" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:15">
       <c r="C20" s="39" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:15">
       <c r="B21" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:15">
       <c r="B22" s="1" t="s">
         <v>19</v>
       </c>
@@ -2214,7 +2283,7 @@
       <c r="N22" s="1"/>
       <c r="O22" s="1"/>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:15">
       <c r="B23" s="1" t="s">
         <v>20</v>
       </c>
@@ -2231,25 +2300,25 @@
       <c r="N23" s="1"/>
       <c r="O23" s="1"/>
     </row>
-    <row r="24" spans="1:15" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:15" ht="14.45" customHeight="1">
       <c r="A24" s="40"/>
-      <c r="B24" s="44" t="s">
+      <c r="B24" s="52" t="s">
         <v>21</v>
       </c>
-      <c r="C24" s="44"/>
-      <c r="D24" s="44"/>
-      <c r="E24" s="44"/>
-      <c r="F24" s="44"/>
-      <c r="G24" s="44"/>
-      <c r="H24" s="44"/>
-      <c r="I24" s="44"/>
-      <c r="J24" s="44"/>
-      <c r="K24" s="44"/>
-      <c r="L24" s="44"/>
-      <c r="M24" s="44"/>
-      <c r="N24" s="44"/>
-    </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="C24" s="52"/>
+      <c r="D24" s="52"/>
+      <c r="E24" s="52"/>
+      <c r="F24" s="52"/>
+      <c r="G24" s="52"/>
+      <c r="H24" s="52"/>
+      <c r="I24" s="52"/>
+      <c r="J24" s="52"/>
+      <c r="K24" s="52"/>
+      <c r="L24" s="52"/>
+      <c r="M24" s="52"/>
+      <c r="N24" s="52"/>
+    </row>
+    <row r="26" spans="1:15">
       <c r="C26" s="42"/>
     </row>
   </sheetData>
@@ -2271,62 +2340,62 @@
   <dimension ref="B1:N22"/>
   <sheetViews>
     <sheetView topLeftCell="B1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8:N12"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="10.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="18.1640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.83203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="5.83203125" customWidth="1"/>
+    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.85546875" customWidth="1"/>
     <col min="7" max="7" width="8" customWidth="1"/>
-    <col min="8" max="8" width="11.83203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="20.5" customWidth="1"/>
-    <col min="11" max="11" width="16.5" customWidth="1"/>
-    <col min="12" max="12" width="12.83203125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="29.5" customWidth="1"/>
+    <col min="8" max="8" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20.42578125" customWidth="1"/>
+    <col min="11" max="11" width="16.42578125" customWidth="1"/>
+    <col min="12" max="12" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="29.42578125" customWidth="1"/>
     <col min="14" max="14" width="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B1" s="45" t="s">
+    <row r="1" spans="2:14">
+      <c r="B1" s="53" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="46"/>
-      <c r="D1" s="46"/>
-      <c r="E1" s="47"/>
-    </row>
-    <row r="3" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B3" s="52" t="s">
-        <v>76</v>
-      </c>
-      <c r="C3" s="53"/>
-      <c r="D3" s="53"/>
-      <c r="E3" s="53"/>
-      <c r="F3" s="53"/>
-      <c r="G3" s="54"/>
-    </row>
-    <row r="5" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B5" s="55" t="s">
+      <c r="C1" s="54"/>
+      <c r="D1" s="54"/>
+      <c r="E1" s="55"/>
+    </row>
+    <row r="3" spans="2:14">
+      <c r="B3" s="74" t="s">
+        <v>74</v>
+      </c>
+      <c r="C3" s="75"/>
+      <c r="D3" s="75"/>
+      <c r="E3" s="75"/>
+      <c r="F3" s="75"/>
+      <c r="G3" s="76"/>
+    </row>
+    <row r="5" spans="2:14">
+      <c r="B5" s="77" t="s">
         <v>22</v>
       </c>
-      <c r="C5" s="55"/>
-      <c r="D5" s="55"/>
-      <c r="E5" s="55"/>
-      <c r="G5" s="56" t="s">
+      <c r="C5" s="77"/>
+      <c r="D5" s="77"/>
+      <c r="E5" s="77"/>
+      <c r="G5" s="78" t="s">
         <v>23</v>
       </c>
-      <c r="H5" s="56"/>
-      <c r="I5" s="56"/>
-      <c r="J5" s="56"/>
-      <c r="K5" s="56"/>
-      <c r="L5" s="56"/>
-      <c r="M5" s="56"/>
-      <c r="N5" s="56"/>
-    </row>
-    <row r="6" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="H5" s="78"/>
+      <c r="I5" s="78"/>
+      <c r="J5" s="78"/>
+      <c r="K5" s="78"/>
+      <c r="L5" s="78"/>
+      <c r="M5" s="78"/>
+      <c r="N5" s="78"/>
+    </row>
+    <row r="6" spans="2:14">
       <c r="B6" s="18" t="s">
         <v>24</v>
       </c>
@@ -2339,60 +2408,58 @@
       <c r="E6" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="G6" s="57" t="s">
+      <c r="G6" s="79" t="s">
         <v>28</v>
       </c>
-      <c r="H6" s="69" t="s">
+      <c r="H6" s="65" t="s">
         <v>29</v>
       </c>
-      <c r="I6" s="67" t="s">
+      <c r="I6" s="68" t="s">
         <v>30</v>
       </c>
-      <c r="J6" s="72"/>
-      <c r="K6" s="72"/>
-      <c r="L6" s="72"/>
-      <c r="M6" s="71" t="s">
+      <c r="J6" s="69"/>
+      <c r="K6" s="69"/>
+      <c r="L6" s="69"/>
+      <c r="M6" s="67" t="s">
         <v>31</v>
       </c>
-      <c r="N6" s="71"/>
-    </row>
-    <row r="7" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="N6" s="67"/>
+    </row>
+    <row r="7" spans="2:14">
       <c r="B7" s="4">
         <v>1</v>
       </c>
-      <c r="C7" s="49" t="s">
-        <v>77</v>
+      <c r="C7" s="73" t="s">
+        <v>75</v>
       </c>
       <c r="D7" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="E7" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="G7" s="58"/>
-      <c r="H7" s="70"/>
+      <c r="E7" s="4"/>
+      <c r="G7" s="80"/>
+      <c r="H7" s="66"/>
       <c r="I7" s="18" t="s">
         <v>33</v>
       </c>
       <c r="J7" s="18" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="K7" s="18" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="L7" s="18" t="s">
-        <v>87</v>
-      </c>
-      <c r="M7" s="67" t="s">
+        <v>84</v>
+      </c>
+      <c r="M7" s="68" t="s">
         <v>34</v>
       </c>
-      <c r="N7" s="68"/>
-    </row>
-    <row r="8" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="N7" s="70"/>
+    </row>
+    <row r="8" spans="2:14">
       <c r="B8" s="4">
         <v>2</v>
       </c>
-      <c r="C8" s="49"/>
+      <c r="C8" s="73"/>
       <c r="D8" s="4"/>
       <c r="E8" s="4" t="s">
         <v>35</v>
@@ -2401,166 +2468,166 @@
         <v>1</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="J8" s="112">
+        <v>85</v>
+      </c>
+      <c r="J8" s="44">
         <v>45385</v>
       </c>
-      <c r="K8" s="112">
+      <c r="K8" s="44">
         <v>45389</v>
       </c>
       <c r="L8" s="2">
         <v>2</v>
       </c>
-      <c r="M8" s="65" t="s">
+      <c r="M8" s="57" t="s">
         <v>36</v>
       </c>
-      <c r="N8" s="66"/>
-    </row>
-    <row r="9" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="N8" s="58"/>
+    </row>
+    <row r="9" spans="2:14">
       <c r="B9" s="4">
         <v>3</v>
       </c>
-      <c r="C9" s="50" t="s">
-        <v>78</v>
+      <c r="C9" s="59" t="s">
+        <v>76</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="E9" s="4"/>
       <c r="G9" s="18">
         <v>2</v>
       </c>
-      <c r="H9" s="113" t="s">
-        <v>90</v>
+      <c r="H9" s="45" t="s">
+        <v>87</v>
       </c>
       <c r="I9" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="J9" s="112">
+      <c r="J9" s="44">
         <v>45385</v>
       </c>
-      <c r="K9" s="112">
+      <c r="K9" s="44">
         <v>45389</v>
       </c>
       <c r="L9" s="2">
         <v>3</v>
       </c>
-      <c r="M9" s="65" t="s">
+      <c r="M9" s="57" t="s">
         <v>41</v>
       </c>
-      <c r="N9" s="66"/>
-    </row>
-    <row r="10" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="N9" s="58"/>
+    </row>
+    <row r="10" spans="2:14">
       <c r="B10" s="4">
         <v>4</v>
       </c>
-      <c r="C10" s="51"/>
+      <c r="C10" s="61"/>
       <c r="D10" s="4"/>
       <c r="E10" s="4" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="G10" s="28">
         <v>3</v>
       </c>
-      <c r="H10" s="114" t="s">
-        <v>91</v>
+      <c r="H10" s="46" t="s">
+        <v>88</v>
       </c>
       <c r="I10" s="10" t="s">
-        <v>92</v>
-      </c>
-      <c r="J10" s="115">
+        <v>89</v>
+      </c>
+      <c r="J10" s="47">
         <v>25328</v>
       </c>
-      <c r="K10" s="115">
+      <c r="K10" s="47">
         <v>45389</v>
       </c>
       <c r="L10" s="10">
         <v>5</v>
       </c>
-      <c r="M10" s="59" t="s">
-        <v>93</v>
-      </c>
-      <c r="N10" s="60"/>
-    </row>
-    <row r="11" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="M10" s="81" t="s">
+        <v>90</v>
+      </c>
+      <c r="N10" s="82"/>
+    </row>
+    <row r="11" spans="2:14" ht="15" customHeight="1">
       <c r="B11" s="4">
         <v>5</v>
       </c>
-      <c r="C11" s="49" t="s">
-        <v>81</v>
+      <c r="C11" s="73" t="s">
+        <v>79</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E11" s="4"/>
       <c r="G11" s="28">
         <v>4</v>
       </c>
       <c r="H11" s="10" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="I11" s="10" t="s">
-        <v>94</v>
-      </c>
-      <c r="J11" s="115">
+        <v>91</v>
+      </c>
+      <c r="J11" s="47">
         <v>45385</v>
       </c>
-      <c r="K11" s="115">
+      <c r="K11" s="47">
         <v>17418</v>
       </c>
       <c r="L11" s="10">
         <v>4</v>
       </c>
-      <c r="M11" s="59" t="s">
-        <v>95</v>
-      </c>
-      <c r="N11" s="60"/>
-    </row>
-    <row r="12" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="M11" s="81" t="s">
+        <v>92</v>
+      </c>
+      <c r="N11" s="82"/>
+    </row>
+    <row r="12" spans="2:14">
       <c r="B12" s="4">
         <v>6</v>
       </c>
-      <c r="C12" s="49"/>
+      <c r="C12" s="73"/>
       <c r="D12" s="4"/>
       <c r="E12" s="4" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="G12" s="9">
         <v>5</v>
       </c>
       <c r="H12" s="6" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="I12" s="6" t="s">
-        <v>98</v>
-      </c>
-      <c r="J12" s="116">
+        <v>95</v>
+      </c>
+      <c r="J12" s="48">
         <v>45385</v>
       </c>
-      <c r="K12" s="116">
+      <c r="K12" s="48">
         <v>45389</v>
       </c>
       <c r="L12" s="6">
         <v>-2</v>
       </c>
-      <c r="M12" s="61" t="s">
-        <v>99</v>
-      </c>
-      <c r="N12" s="62"/>
-    </row>
-    <row r="13" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="M12" s="71" t="s">
+        <v>96</v>
+      </c>
+      <c r="N12" s="72"/>
+    </row>
+    <row r="13" spans="2:14">
       <c r="B13" s="4">
         <v>7</v>
       </c>
-      <c r="C13" s="50" t="s">
-        <v>108</v>
+      <c r="C13" s="59" t="s">
+        <v>105</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="E13" s="4"/>
       <c r="G13" s="9"/>
@@ -2569,16 +2636,16 @@
       <c r="J13" s="6"/>
       <c r="K13" s="6"/>
       <c r="L13" s="6"/>
-      <c r="M13" s="61"/>
-      <c r="N13" s="62"/>
-    </row>
-    <row r="14" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="M13" s="71"/>
+      <c r="N13" s="72"/>
+    </row>
+    <row r="14" spans="2:14">
       <c r="B14" s="4">
         <v>8</v>
       </c>
-      <c r="C14" s="74"/>
+      <c r="C14" s="60"/>
       <c r="D14" s="4" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="E14" s="4"/>
       <c r="G14" s="14"/>
@@ -2590,14 +2657,14 @@
       <c r="M14" s="63"/>
       <c r="N14" s="64"/>
     </row>
-    <row r="15" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:14">
       <c r="B15" s="4">
         <v>9</v>
       </c>
-      <c r="C15" s="51"/>
+      <c r="C15" s="61"/>
       <c r="D15" s="4"/>
       <c r="E15" s="4" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="G15" s="14"/>
       <c r="H15" s="13"/>
@@ -2608,7 +2675,7 @@
       <c r="M15" s="63"/>
       <c r="N15" s="64"/>
     </row>
-    <row r="16" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:14">
       <c r="B16" s="4">
         <v>10</v>
       </c>
@@ -2624,11 +2691,11 @@
       <c r="M16" s="63"/>
       <c r="N16" s="64"/>
     </row>
-    <row r="17" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:14">
       <c r="B17" s="4">
         <v>11</v>
       </c>
-      <c r="C17" s="49" t="s">
+      <c r="C17" s="73" t="s">
         <v>37</v>
       </c>
       <c r="D17" s="4"/>
@@ -2642,11 +2709,11 @@
       <c r="M17" s="63"/>
       <c r="N17" s="64"/>
     </row>
-    <row r="18" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:14">
       <c r="B18" s="4">
         <v>12</v>
       </c>
-      <c r="C18" s="49"/>
+      <c r="C18" s="73"/>
       <c r="D18" s="4"/>
       <c r="E18" s="4"/>
       <c r="G18" s="14"/>
@@ -2658,11 +2725,11 @@
       <c r="M18" s="63"/>
       <c r="N18" s="64"/>
     </row>
-    <row r="19" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:14">
       <c r="B19" s="4">
         <v>13</v>
       </c>
-      <c r="C19" s="49" t="s">
+      <c r="C19" s="73" t="s">
         <v>37</v>
       </c>
       <c r="D19" s="4"/>
@@ -2676,38 +2743,23 @@
       <c r="M19" s="63"/>
       <c r="N19" s="64"/>
     </row>
-    <row r="20" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:14">
       <c r="B20" s="4">
         <v>14</v>
       </c>
-      <c r="C20" s="49"/>
+      <c r="C20" s="73"/>
       <c r="D20" s="4"/>
       <c r="E20" s="4"/>
     </row>
-    <row r="22" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:14">
       <c r="D22" t="s">
         <v>42</v>
       </c>
-      <c r="F22" s="73"/>
-      <c r="G22" s="73"/>
+      <c r="F22" s="62"/>
+      <c r="G22" s="62"/>
     </row>
   </sheetData>
   <mergeCells count="28">
-    <mergeCell ref="M9:N9"/>
-    <mergeCell ref="C13:C15"/>
-    <mergeCell ref="F22:G22"/>
-    <mergeCell ref="M16:N16"/>
-    <mergeCell ref="M17:N17"/>
-    <mergeCell ref="M18:N18"/>
-    <mergeCell ref="M19:N19"/>
-    <mergeCell ref="M15:N15"/>
-    <mergeCell ref="M8:N8"/>
-    <mergeCell ref="H6:H7"/>
-    <mergeCell ref="M6:N6"/>
-    <mergeCell ref="I6:L6"/>
-    <mergeCell ref="M7:N7"/>
-    <mergeCell ref="M13:N13"/>
-    <mergeCell ref="M14:N14"/>
     <mergeCell ref="B1:E1"/>
     <mergeCell ref="C19:C20"/>
     <mergeCell ref="C7:C8"/>
@@ -2721,6 +2773,21 @@
     <mergeCell ref="M10:N10"/>
     <mergeCell ref="M11:N11"/>
     <mergeCell ref="M12:N12"/>
+    <mergeCell ref="M8:N8"/>
+    <mergeCell ref="H6:H7"/>
+    <mergeCell ref="M6:N6"/>
+    <mergeCell ref="I6:L6"/>
+    <mergeCell ref="M7:N7"/>
+    <mergeCell ref="M9:N9"/>
+    <mergeCell ref="C13:C15"/>
+    <mergeCell ref="F22:G22"/>
+    <mergeCell ref="M16:N16"/>
+    <mergeCell ref="M17:N17"/>
+    <mergeCell ref="M18:N18"/>
+    <mergeCell ref="M19:N19"/>
+    <mergeCell ref="M15:N15"/>
+    <mergeCell ref="M13:N13"/>
+    <mergeCell ref="M14:N14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2737,63 +2804,63 @@
       <selection activeCell="K8" sqref="K8:P15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="30.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="30.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="7" customWidth="1"/>
-    <col min="6" max="6" width="5.5" customWidth="1"/>
-    <col min="7" max="7" width="9.5" customWidth="1"/>
+    <col min="6" max="6" width="5.42578125" customWidth="1"/>
+    <col min="7" max="7" width="9.42578125" customWidth="1"/>
     <col min="9" max="9" width="10" customWidth="1"/>
-    <col min="10" max="10" width="10.1640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.5" customWidth="1"/>
-    <col min="12" max="12" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="7.33203125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="12.83203125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="23.33203125" customWidth="1"/>
-    <col min="16" max="16" width="9.5" customWidth="1"/>
+    <col min="10" max="10" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.42578125" customWidth="1"/>
+    <col min="12" max="12" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="23.28515625" customWidth="1"/>
+    <col min="16" max="16" width="9.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B1" s="45" t="s">
+    <row r="1" spans="2:16">
+      <c r="B1" s="53" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="46"/>
-      <c r="D1" s="46"/>
-      <c r="E1" s="47"/>
-    </row>
-    <row r="3" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B3" s="52" t="s">
+      <c r="C1" s="54"/>
+      <c r="D1" s="54"/>
+      <c r="E1" s="55"/>
+    </row>
+    <row r="3" spans="2:16">
+      <c r="B3" s="74" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="53"/>
-      <c r="D3" s="53"/>
-      <c r="E3" s="53"/>
-      <c r="F3" s="53"/>
-      <c r="G3" s="54"/>
-    </row>
-    <row r="5" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B5" s="80" t="s">
+      <c r="C3" s="75"/>
+      <c r="D3" s="75"/>
+      <c r="E3" s="75"/>
+      <c r="F3" s="75"/>
+      <c r="G3" s="76"/>
+    </row>
+    <row r="5" spans="2:16">
+      <c r="B5" s="88" t="s">
         <v>43</v>
       </c>
-      <c r="C5" s="80"/>
-      <c r="D5" s="80"/>
+      <c r="C5" s="88"/>
+      <c r="D5" s="88"/>
       <c r="E5" s="3"/>
-      <c r="G5" s="56" t="s">
+      <c r="G5" s="78" t="s">
         <v>44</v>
       </c>
-      <c r="H5" s="56"/>
-      <c r="I5" s="56"/>
-      <c r="J5" s="56"/>
-      <c r="K5" s="56"/>
-      <c r="L5" s="56"/>
-      <c r="M5" s="56"/>
-      <c r="N5" s="56"/>
-      <c r="O5" s="56"/>
-      <c r="P5" s="56"/>
-    </row>
-    <row r="6" spans="2:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H5" s="78"/>
+      <c r="I5" s="78"/>
+      <c r="J5" s="78"/>
+      <c r="K5" s="78"/>
+      <c r="L5" s="78"/>
+      <c r="M5" s="78"/>
+      <c r="N5" s="78"/>
+      <c r="O5" s="78"/>
+      <c r="P5" s="78"/>
+    </row>
+    <row r="6" spans="2:16" ht="14.45" customHeight="1">
       <c r="B6" s="4" t="s">
         <v>45</v>
       </c>
@@ -2804,65 +2871,65 @@
         <v>43</v>
       </c>
       <c r="E6" s="7"/>
-      <c r="G6" s="57" t="s">
+      <c r="G6" s="79" t="s">
         <v>46</v>
       </c>
-      <c r="H6" s="57" t="s">
+      <c r="H6" s="79" t="s">
         <v>47</v>
       </c>
-      <c r="I6" s="57" t="s">
+      <c r="I6" s="79" t="s">
         <v>48</v>
       </c>
-      <c r="J6" s="69" t="s">
+      <c r="J6" s="65" t="s">
         <v>49</v>
       </c>
-      <c r="K6" s="81" t="s">
+      <c r="K6" s="85" t="s">
         <v>30</v>
       </c>
-      <c r="L6" s="85"/>
-      <c r="M6" s="85"/>
-      <c r="N6" s="85"/>
-      <c r="O6" s="81" t="s">
+      <c r="L6" s="86"/>
+      <c r="M6" s="86"/>
+      <c r="N6" s="86"/>
+      <c r="O6" s="85" t="s">
         <v>31</v>
       </c>
-      <c r="P6" s="82"/>
-    </row>
-    <row r="7" spans="2:16" ht="16" x14ac:dyDescent="0.2">
-      <c r="B7" s="50">
+      <c r="P6" s="89"/>
+    </row>
+    <row r="7" spans="2:16">
+      <c r="B7" s="59">
         <v>1</v>
       </c>
-      <c r="C7" s="75" t="s">
-        <v>112</v>
+      <c r="C7" s="90" t="s">
+        <v>109</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="G7" s="58"/>
-      <c r="H7" s="58"/>
-      <c r="I7" s="58"/>
-      <c r="J7" s="70"/>
+        <v>111</v>
+      </c>
+      <c r="G7" s="80"/>
+      <c r="H7" s="80"/>
+      <c r="I7" s="80"/>
+      <c r="J7" s="66"/>
       <c r="K7" s="18" t="s">
         <v>33</v>
       </c>
       <c r="L7" s="18" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="M7" s="27" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="N7" s="27" t="s">
-        <v>87</v>
-      </c>
-      <c r="O7" s="67" t="s">
+        <v>84</v>
+      </c>
+      <c r="O7" s="68" t="s">
         <v>50</v>
       </c>
-      <c r="P7" s="68"/>
-    </row>
-    <row r="8" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B8" s="74"/>
-      <c r="C8" s="76"/>
+      <c r="P7" s="70"/>
+    </row>
+    <row r="8" spans="2:16">
+      <c r="B8" s="60"/>
+      <c r="C8" s="91"/>
       <c r="D8" s="4" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="G8" s="18">
         <v>1</v>
@@ -2872,15 +2939,15 @@
       </c>
       <c r="I8" s="11"/>
       <c r="J8" s="11" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="K8" s="26" t="s">
-        <v>107</v>
-      </c>
-      <c r="L8" s="117">
+        <v>104</v>
+      </c>
+      <c r="L8" s="49">
         <v>25601</v>
       </c>
-      <c r="M8" s="117">
+      <c r="M8" s="49">
         <v>25602</v>
       </c>
       <c r="N8" s="26">
@@ -2891,11 +2958,11 @@
       </c>
       <c r="P8" s="84"/>
     </row>
-    <row r="9" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B9" s="74"/>
-      <c r="C9" s="76"/>
+    <row r="9" spans="2:16">
+      <c r="B9" s="60"/>
+      <c r="C9" s="91"/>
       <c r="D9" s="4" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="G9" s="14">
         <v>2</v>
@@ -2905,30 +2972,30 @@
       </c>
       <c r="I9" s="16"/>
       <c r="J9" s="16" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="K9" s="17" t="s">
-        <v>116</v>
-      </c>
-      <c r="L9" s="118">
+        <v>113</v>
+      </c>
+      <c r="L9" s="50">
         <v>25601</v>
       </c>
-      <c r="M9" s="118">
+      <c r="M9" s="50">
         <v>25602</v>
       </c>
       <c r="N9" s="13" t="s">
-        <v>117</v>
-      </c>
-      <c r="O9" s="61" t="s">
+        <v>114</v>
+      </c>
+      <c r="O9" s="71" t="s">
         <v>36</v>
       </c>
-      <c r="P9" s="62"/>
-    </row>
-    <row r="10" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B10" s="74"/>
-      <c r="C10" s="76"/>
-      <c r="D10" s="50" t="s">
-        <v>101</v>
+      <c r="P9" s="72"/>
+    </row>
+    <row r="10" spans="2:16">
+      <c r="B10" s="60"/>
+      <c r="C10" s="91"/>
+      <c r="D10" s="59" t="s">
+        <v>98</v>
       </c>
       <c r="G10" s="18">
         <v>3</v>
@@ -2938,29 +3005,29 @@
       </c>
       <c r="I10" s="11"/>
       <c r="J10" s="11" t="s">
+        <v>112</v>
+      </c>
+      <c r="K10" s="25" t="s">
         <v>115</v>
       </c>
-      <c r="K10" s="25" t="s">
-        <v>118</v>
-      </c>
-      <c r="L10" s="117">
+      <c r="L10" s="49">
         <v>25601</v>
       </c>
-      <c r="M10" s="117">
+      <c r="M10" s="49">
         <v>25602</v>
       </c>
       <c r="N10" s="26">
         <v>0</v>
       </c>
       <c r="O10" s="83" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="P10" s="84"/>
     </row>
-    <row r="11" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B11" s="74"/>
-      <c r="C11" s="76"/>
-      <c r="D11" s="74"/>
+    <row r="11" spans="2:16">
+      <c r="B11" s="60"/>
+      <c r="C11" s="91"/>
+      <c r="D11" s="60"/>
       <c r="G11" s="18">
         <v>4</v>
       </c>
@@ -2969,29 +3036,29 @@
       </c>
       <c r="I11" s="11"/>
       <c r="J11" s="11" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="K11" s="25" t="s">
-        <v>119</v>
-      </c>
-      <c r="L11" s="117">
+        <v>116</v>
+      </c>
+      <c r="L11" s="49">
         <v>25601</v>
       </c>
-      <c r="M11" s="117">
+      <c r="M11" s="49">
         <v>25602</v>
       </c>
       <c r="N11" s="26">
         <v>-1</v>
       </c>
       <c r="O11" s="83" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="P11" s="84"/>
     </row>
-    <row r="12" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B12" s="51"/>
-      <c r="C12" s="77"/>
-      <c r="D12" s="51"/>
+    <row r="12" spans="2:16">
+      <c r="B12" s="61"/>
+      <c r="C12" s="92"/>
+      <c r="D12" s="61"/>
       <c r="G12" s="18">
         <v>5</v>
       </c>
@@ -3000,16 +3067,16 @@
       </c>
       <c r="I12" s="11"/>
       <c r="J12" s="11" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="K12" s="25" t="s">
-        <v>120</v>
-      </c>
-      <c r="L12" s="117">
+        <v>117</v>
+      </c>
+      <c r="L12" s="49">
         <v>25569</v>
       </c>
       <c r="M12" s="26" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="N12" s="26">
         <v>2</v>
@@ -3019,15 +3086,15 @@
       </c>
       <c r="P12" s="84"/>
     </row>
-    <row r="13" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B13" s="50">
+    <row r="13" spans="2:16">
+      <c r="B13" s="59">
         <v>2</v>
       </c>
-      <c r="C13" s="50" t="s">
-        <v>102</v>
+      <c r="C13" s="59" t="s">
+        <v>99</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="G13" s="14">
         <v>6</v>
@@ -3037,30 +3104,30 @@
       </c>
       <c r="I13" s="16"/>
       <c r="J13" s="16" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="K13" s="17" t="s">
-        <v>122</v>
-      </c>
-      <c r="L13" s="118">
+        <v>119</v>
+      </c>
+      <c r="L13" s="50">
         <v>25568</v>
       </c>
-      <c r="M13" s="118">
+      <c r="M13" s="50">
         <v>25602</v>
       </c>
       <c r="N13" s="13">
         <v>4</v>
       </c>
-      <c r="O13" s="61" t="s">
-        <v>123</v>
-      </c>
-      <c r="P13" s="62"/>
-    </row>
-    <row r="14" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B14" s="74"/>
-      <c r="C14" s="74"/>
+      <c r="O13" s="71" t="s">
+        <v>120</v>
+      </c>
+      <c r="P13" s="72"/>
+    </row>
+    <row r="14" spans="2:16">
+      <c r="B14" s="60"/>
+      <c r="C14" s="60"/>
       <c r="D14" s="4" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="G14" s="18">
         <v>7</v>
@@ -3070,15 +3137,15 @@
       </c>
       <c r="I14" s="11"/>
       <c r="J14" s="11" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="K14" s="26" t="s">
-        <v>124</v>
-      </c>
-      <c r="L14" s="117">
+        <v>121</v>
+      </c>
+      <c r="L14" s="49">
         <v>25935</v>
       </c>
-      <c r="M14" s="117">
+      <c r="M14" s="49">
         <v>25602</v>
       </c>
       <c r="N14" s="26">
@@ -3089,11 +3156,11 @@
       </c>
       <c r="P14" s="84"/>
     </row>
-    <row r="15" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B15" s="74"/>
-      <c r="C15" s="74"/>
+    <row r="15" spans="2:16">
+      <c r="B15" s="60"/>
+      <c r="C15" s="60"/>
       <c r="D15" s="4" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="G15" s="18">
         <v>8</v>
@@ -3103,30 +3170,30 @@
       </c>
       <c r="I15" s="11"/>
       <c r="J15" s="11" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="K15" s="26" t="s">
-        <v>125</v>
-      </c>
-      <c r="L15" s="117">
+        <v>122</v>
+      </c>
+      <c r="L15" s="49">
         <v>25202</v>
       </c>
-      <c r="M15" s="117">
+      <c r="M15" s="49">
         <v>25602</v>
       </c>
       <c r="N15" s="26">
         <v>99</v>
       </c>
       <c r="O15" s="83" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="P15" s="84"/>
     </row>
-    <row r="16" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B16" s="74"/>
-      <c r="C16" s="74"/>
-      <c r="D16" s="50" t="s">
-        <v>105</v>
+    <row r="16" spans="2:16">
+      <c r="B16" s="60"/>
+      <c r="C16" s="60"/>
+      <c r="D16" s="59" t="s">
+        <v>102</v>
       </c>
       <c r="G16" s="18">
         <v>9</v>
@@ -3140,10 +3207,10 @@
       <c r="O16" s="83"/>
       <c r="P16" s="84"/>
     </row>
-    <row r="17" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B17" s="74"/>
-      <c r="C17" s="74"/>
-      <c r="D17" s="74"/>
+    <row r="17" spans="2:16">
+      <c r="B17" s="60"/>
+      <c r="C17" s="60"/>
+      <c r="D17" s="60"/>
       <c r="G17" s="18">
         <v>10</v>
       </c>
@@ -3157,10 +3224,10 @@
       <c r="O17" s="83"/>
       <c r="P17" s="84"/>
     </row>
-    <row r="18" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B18" s="51"/>
-      <c r="C18" s="51"/>
-      <c r="D18" s="51"/>
+    <row r="18" spans="2:16">
+      <c r="B18" s="61"/>
+      <c r="C18" s="61"/>
+      <c r="D18" s="61"/>
       <c r="G18" s="18">
         <v>11</v>
       </c>
@@ -3174,11 +3241,11 @@
       <c r="O18" s="83"/>
       <c r="P18" s="84"/>
     </row>
-    <row r="19" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B19" s="50">
+    <row r="19" spans="2:16">
+      <c r="B19" s="59">
         <v>3</v>
       </c>
-      <c r="C19" s="75"/>
+      <c r="C19" s="90"/>
       <c r="D19" s="2"/>
       <c r="G19" s="18">
         <v>12</v>
@@ -3193,9 +3260,9 @@
       <c r="O19" s="83"/>
       <c r="P19" s="84"/>
     </row>
-    <row r="20" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B20" s="74"/>
-      <c r="C20" s="76"/>
+    <row r="20" spans="2:16">
+      <c r="B20" s="60"/>
+      <c r="C20" s="91"/>
       <c r="D20" s="2"/>
       <c r="G20" s="18">
         <v>13</v>
@@ -3210,9 +3277,9 @@
       <c r="O20" s="83"/>
       <c r="P20" s="84"/>
     </row>
-    <row r="21" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B21" s="74"/>
-      <c r="C21" s="76"/>
+    <row r="21" spans="2:16">
+      <c r="B21" s="60"/>
+      <c r="C21" s="91"/>
       <c r="D21" s="2"/>
       <c r="G21" s="18">
         <v>14</v>
@@ -3227,9 +3294,9 @@
       <c r="O21" s="83"/>
       <c r="P21" s="84"/>
     </row>
-    <row r="22" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B22" s="74"/>
-      <c r="C22" s="76"/>
+    <row r="22" spans="2:16">
+      <c r="B22" s="60"/>
+      <c r="C22" s="91"/>
       <c r="D22" s="2"/>
       <c r="G22" s="18">
         <v>15</v>
@@ -3244,9 +3311,9 @@
       <c r="O22" s="83"/>
       <c r="P22" s="84"/>
     </row>
-    <row r="23" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B23" s="74"/>
-      <c r="C23" s="76"/>
+    <row r="23" spans="2:16">
+      <c r="B23" s="60"/>
+      <c r="C23" s="91"/>
       <c r="D23" s="2"/>
       <c r="G23" s="18">
         <v>16</v>
@@ -3261,9 +3328,9 @@
       <c r="O23" s="83"/>
       <c r="P23" s="84"/>
     </row>
-    <row r="24" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B24" s="51"/>
-      <c r="C24" s="77"/>
+    <row r="24" spans="2:16">
+      <c r="B24" s="61"/>
+      <c r="C24" s="92"/>
       <c r="D24" s="2"/>
       <c r="G24" s="18">
         <v>17</v>
@@ -3278,11 +3345,11 @@
       <c r="O24" s="83"/>
       <c r="P24" s="84"/>
     </row>
-    <row r="25" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B25" s="50">
+    <row r="25" spans="2:16">
+      <c r="B25" s="59">
         <v>4</v>
       </c>
-      <c r="C25" s="75"/>
+      <c r="C25" s="90"/>
       <c r="D25" s="2"/>
       <c r="G25" s="18">
         <v>18</v>
@@ -3297,73 +3364,47 @@
       <c r="O25" s="83"/>
       <c r="P25" s="84"/>
     </row>
-    <row r="26" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B26" s="74"/>
-      <c r="C26" s="76"/>
+    <row r="26" spans="2:16">
+      <c r="B26" s="60"/>
+      <c r="C26" s="91"/>
       <c r="D26" s="2"/>
     </row>
-    <row r="27" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B27" s="74"/>
-      <c r="C27" s="76"/>
+    <row r="27" spans="2:16">
+      <c r="B27" s="60"/>
+      <c r="C27" s="91"/>
       <c r="D27" s="2"/>
     </row>
-    <row r="28" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B28" s="74"/>
-      <c r="C28" s="76"/>
+    <row r="28" spans="2:16">
+      <c r="B28" s="60"/>
+      <c r="C28" s="91"/>
       <c r="D28" s="2"/>
-      <c r="G28" s="73"/>
-      <c r="H28" s="73"/>
-      <c r="I28" s="79"/>
-      <c r="J28" s="79"/>
-      <c r="K28" s="79"/>
-      <c r="L28" s="79"/>
-      <c r="M28" s="79"/>
+      <c r="G28" s="62"/>
+      <c r="H28" s="62"/>
+      <c r="I28" s="87"/>
+      <c r="J28" s="87"/>
+      <c r="K28" s="87"/>
+      <c r="L28" s="87"/>
+      <c r="M28" s="87"/>
       <c r="N28" s="35"/>
     </row>
-    <row r="29" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B29" s="74"/>
-      <c r="C29" s="76"/>
+    <row r="29" spans="2:16">
+      <c r="B29" s="60"/>
+      <c r="C29" s="91"/>
       <c r="D29" s="2"/>
-      <c r="I29" s="78"/>
-      <c r="J29" s="78"/>
-      <c r="K29" s="78"/>
-      <c r="L29" s="78"/>
-      <c r="M29" s="78"/>
+      <c r="I29" s="93"/>
+      <c r="J29" s="93"/>
+      <c r="K29" s="93"/>
+      <c r="L29" s="93"/>
+      <c r="M29" s="93"/>
       <c r="N29" s="36"/>
     </row>
-    <row r="30" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B30" s="51"/>
-      <c r="C30" s="77"/>
+    <row r="30" spans="2:16">
+      <c r="B30" s="61"/>
+      <c r="C30" s="92"/>
       <c r="D30" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="42">
-    <mergeCell ref="D10:D12"/>
-    <mergeCell ref="D16:D18"/>
-    <mergeCell ref="O19:P19"/>
-    <mergeCell ref="O20:P20"/>
-    <mergeCell ref="O21:P21"/>
-    <mergeCell ref="O13:P13"/>
-    <mergeCell ref="K6:N6"/>
-    <mergeCell ref="O10:P10"/>
-    <mergeCell ref="O11:P11"/>
-    <mergeCell ref="O12:P12"/>
-    <mergeCell ref="G28:H28"/>
-    <mergeCell ref="I28:M28"/>
-    <mergeCell ref="B5:D5"/>
-    <mergeCell ref="O6:P6"/>
-    <mergeCell ref="H6:H7"/>
-    <mergeCell ref="O25:P25"/>
-    <mergeCell ref="O14:P14"/>
-    <mergeCell ref="O15:P15"/>
-    <mergeCell ref="O22:P22"/>
-    <mergeCell ref="O23:P23"/>
-    <mergeCell ref="O24:P24"/>
-    <mergeCell ref="O16:P16"/>
-    <mergeCell ref="O17:P17"/>
-    <mergeCell ref="O18:P18"/>
-    <mergeCell ref="O8:P8"/>
-    <mergeCell ref="O9:P9"/>
     <mergeCell ref="B1:E1"/>
     <mergeCell ref="G6:G7"/>
     <mergeCell ref="I6:I7"/>
@@ -3380,6 +3421,32 @@
     <mergeCell ref="G5:P5"/>
     <mergeCell ref="B3:G3"/>
     <mergeCell ref="O7:P7"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="O6:P6"/>
+    <mergeCell ref="H6:H7"/>
+    <mergeCell ref="O25:P25"/>
+    <mergeCell ref="O14:P14"/>
+    <mergeCell ref="O15:P15"/>
+    <mergeCell ref="O22:P22"/>
+    <mergeCell ref="O23:P23"/>
+    <mergeCell ref="O24:P24"/>
+    <mergeCell ref="O16:P16"/>
+    <mergeCell ref="O17:P17"/>
+    <mergeCell ref="O18:P18"/>
+    <mergeCell ref="O8:P8"/>
+    <mergeCell ref="O9:P9"/>
+    <mergeCell ref="K6:N6"/>
+    <mergeCell ref="O10:P10"/>
+    <mergeCell ref="O11:P11"/>
+    <mergeCell ref="O12:P12"/>
+    <mergeCell ref="G28:H28"/>
+    <mergeCell ref="I28:M28"/>
+    <mergeCell ref="D10:D12"/>
+    <mergeCell ref="D16:D18"/>
+    <mergeCell ref="O19:P19"/>
+    <mergeCell ref="O20:P20"/>
+    <mergeCell ref="O21:P21"/>
+    <mergeCell ref="O13:P13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3394,43 +3461,45 @@
   </sheetPr>
   <dimension ref="B1:AB26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J30" sqref="J30"/>
+    <sheetView tabSelected="1" topLeftCell="F6" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="Y9" sqref="Y9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="6" max="6" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.5" customWidth="1"/>
-    <col min="9" max="9" width="13.1640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="30.33203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.83203125" customWidth="1"/>
+    <col min="4" max="4" width="17.28515625" customWidth="1"/>
+    <col min="5" max="5" width="24.5703125" customWidth="1"/>
+    <col min="6" max="6" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.5703125" customWidth="1"/>
+    <col min="9" max="9" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="30.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:28" x14ac:dyDescent="0.2">
-      <c r="B1" s="45" t="s">
+    <row r="1" spans="2:28">
+      <c r="B1" s="53" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="46"/>
-      <c r="D1" s="46"/>
-      <c r="E1" s="47"/>
-    </row>
-    <row r="3" spans="2:28" x14ac:dyDescent="0.2">
-      <c r="B3" s="89" t="s">
+      <c r="C1" s="54"/>
+      <c r="D1" s="54"/>
+      <c r="E1" s="55"/>
+    </row>
+    <row r="3" spans="2:28">
+      <c r="B3" s="119" t="s">
         <v>51</v>
       </c>
-      <c r="C3" s="89"/>
-      <c r="D3" s="89"/>
-      <c r="E3" s="89"/>
-      <c r="F3" s="89"/>
-      <c r="G3" s="89"/>
-      <c r="H3" s="89"/>
-      <c r="I3" s="89"/>
-      <c r="J3" s="89"/>
-      <c r="K3" s="89"/>
+      <c r="C3" s="119"/>
+      <c r="D3" s="119"/>
+      <c r="E3" s="119"/>
+      <c r="F3" s="119"/>
+      <c r="G3" s="119"/>
+      <c r="H3" s="119"/>
+      <c r="I3" s="119"/>
+      <c r="J3" s="119"/>
+      <c r="K3" s="119"/>
       <c r="N3" s="21" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="O3" s="21"/>
       <c r="P3" s="22"/>
@@ -3440,51 +3509,51 @@
       <c r="T3" s="5"/>
       <c r="U3" s="5"/>
       <c r="V3" s="5"/>
-      <c r="W3" s="90"/>
-      <c r="X3" s="90"/>
+      <c r="W3" s="102"/>
+      <c r="X3" s="102"/>
       <c r="Y3" s="5"/>
     </row>
-    <row r="4" spans="2:28" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="57" t="s">
+    <row r="4" spans="2:28" ht="15.75" thickBot="1">
+      <c r="B4" s="79" t="s">
         <v>52</v>
       </c>
-      <c r="C4" s="87" t="s">
+      <c r="C4" s="117" t="s">
         <v>53</v>
       </c>
-      <c r="D4" s="93" t="s">
+      <c r="D4" s="105" t="s">
         <v>54</v>
       </c>
-      <c r="E4" s="69" t="s">
+      <c r="E4" s="65" t="s">
         <v>55</v>
       </c>
-      <c r="F4" s="67" t="s">
+      <c r="F4" s="68" t="s">
         <v>30</v>
       </c>
-      <c r="G4" s="72"/>
-      <c r="H4" s="72"/>
-      <c r="I4" s="72"/>
-      <c r="J4" s="71" t="s">
+      <c r="G4" s="69"/>
+      <c r="H4" s="69"/>
+      <c r="I4" s="69"/>
+      <c r="J4" s="67" t="s">
         <v>31</v>
       </c>
-      <c r="K4" s="71"/>
+      <c r="K4" s="67"/>
       <c r="Y4" s="5"/>
     </row>
-    <row r="5" spans="2:28" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="92"/>
-      <c r="C5" s="88"/>
-      <c r="D5" s="94"/>
-      <c r="E5" s="86"/>
+    <row r="5" spans="2:28" ht="16.5" thickTop="1" thickBot="1">
+      <c r="B5" s="104"/>
+      <c r="C5" s="118"/>
+      <c r="D5" s="106"/>
+      <c r="E5" s="116"/>
       <c r="F5" s="20" t="s">
         <v>33</v>
       </c>
       <c r="G5" s="20" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="H5" s="20" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="I5" s="20" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="J5" s="20" t="s">
         <v>34</v>
@@ -3492,478 +3561,482 @@
       <c r="K5" s="20" t="s">
         <v>56</v>
       </c>
-      <c r="O5" s="101" t="s">
+      <c r="O5" s="96" t="s">
+        <v>61</v>
+      </c>
+      <c r="P5" s="98"/>
+      <c r="Q5" s="98"/>
+      <c r="R5" s="99"/>
+      <c r="S5" s="31" t="s">
         <v>62</v>
       </c>
-      <c r="P5" s="102"/>
-      <c r="Q5" s="102"/>
-      <c r="R5" s="103"/>
-      <c r="S5" s="31" t="s">
+      <c r="T5" s="96" t="s">
         <v>63</v>
       </c>
-      <c r="T5" s="101" t="s">
+      <c r="U5" s="97"/>
+      <c r="V5" s="98"/>
+      <c r="W5" s="98"/>
+      <c r="X5" s="99"/>
+      <c r="Y5" s="96" t="s">
         <v>64</v>
       </c>
-      <c r="U5" s="104"/>
-      <c r="V5" s="102"/>
-      <c r="W5" s="102"/>
-      <c r="X5" s="103"/>
-      <c r="Y5" s="101" t="s">
-        <v>65</v>
-      </c>
-      <c r="Z5" s="104"/>
-      <c r="AA5" s="102"/>
-      <c r="AB5" s="103"/>
-    </row>
-    <row r="6" spans="2:28" ht="16" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="Z5" s="97"/>
+      <c r="AA5" s="98"/>
+      <c r="AB5" s="99"/>
+    </row>
+    <row r="6" spans="2:28" ht="15.75" thickTop="1">
       <c r="B6" s="19">
         <v>1</v>
       </c>
-      <c r="C6" s="91" t="s">
+      <c r="C6" s="103" t="s">
         <v>57</v>
       </c>
       <c r="D6" s="23" t="s">
-        <v>58</v>
+        <v>130</v>
       </c>
       <c r="E6" s="19" t="s">
         <v>39</v>
       </c>
-      <c r="F6" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="G6" s="112">
-        <v>45385</v>
-      </c>
-      <c r="H6" s="112">
-        <v>45389</v>
-      </c>
-      <c r="I6" s="2">
-        <v>2</v>
-      </c>
-      <c r="J6" s="65" t="s">
+      <c r="F6" s="120" t="s">
+        <v>132</v>
+      </c>
+      <c r="G6" s="121">
+        <v>37915</v>
+      </c>
+      <c r="H6" s="121">
+        <v>44844</v>
+      </c>
+      <c r="I6" s="120">
+        <v>5</v>
+      </c>
+      <c r="J6" s="122" t="s">
         <v>36</v>
       </c>
-      <c r="K6" s="66"/>
-      <c r="N6" s="97" t="s">
+      <c r="K6" s="123"/>
+      <c r="N6" s="109" t="s">
         <v>53</v>
       </c>
-      <c r="O6" s="98" t="s">
+      <c r="O6" s="110" t="s">
+        <v>65</v>
+      </c>
+      <c r="P6" s="95" t="s">
         <v>66</v>
       </c>
-      <c r="P6" s="99" t="s">
+      <c r="Q6" s="95" t="s">
         <v>67</v>
       </c>
-      <c r="Q6" s="99" t="s">
+      <c r="R6" s="94" t="s">
         <v>68</v>
       </c>
-      <c r="R6" s="100" t="s">
+      <c r="S6" s="115" t="s">
         <v>69</v>
       </c>
-      <c r="S6" s="109" t="s">
+      <c r="T6" s="111" t="s">
         <v>70</v>
       </c>
-      <c r="T6" s="105" t="s">
-        <v>71</v>
-      </c>
-      <c r="U6" s="106"/>
-      <c r="V6" s="99" t="s">
+      <c r="U6" s="112"/>
+      <c r="V6" s="95" t="s">
+        <v>65</v>
+      </c>
+      <c r="W6" s="95" t="s">
         <v>66</v>
       </c>
-      <c r="W6" s="99" t="s">
+      <c r="X6" s="94" t="s">
         <v>67</v>
       </c>
-      <c r="X6" s="100" t="s">
-        <v>68</v>
-      </c>
-      <c r="Y6" s="110" t="s">
-        <v>71</v>
-      </c>
-      <c r="Z6" s="99" t="s">
+      <c r="Y6" s="100" t="s">
+        <v>70</v>
+      </c>
+      <c r="Z6" s="95" t="s">
+        <v>65</v>
+      </c>
+      <c r="AA6" s="95" t="s">
         <v>66</v>
       </c>
-      <c r="AA6" s="99" t="s">
+      <c r="AB6" s="94" t="s">
         <v>67</v>
       </c>
-      <c r="AB6" s="100" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="7" spans="2:28" x14ac:dyDescent="0.2">
+    </row>
+    <row r="7" spans="2:28">
       <c r="B7" s="8">
         <f>B6+1</f>
         <v>2</v>
       </c>
-      <c r="C7" s="91"/>
+      <c r="C7" s="103"/>
       <c r="D7" s="24" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E7" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="F7" s="2" t="s">
+      <c r="F7" s="120" t="s">
         <v>40</v>
       </c>
-      <c r="G7" s="112">
+      <c r="G7" s="121">
         <v>45385</v>
       </c>
-      <c r="H7" s="112">
+      <c r="H7" s="121">
         <v>45389</v>
       </c>
-      <c r="I7" s="2">
+      <c r="I7" s="120">
         <v>3</v>
       </c>
-      <c r="J7" s="65" t="s">
+      <c r="J7" s="122" t="s">
         <v>41</v>
       </c>
-      <c r="K7" s="66"/>
-      <c r="N7" s="97"/>
-      <c r="O7" s="98"/>
-      <c r="P7" s="99"/>
-      <c r="Q7" s="99"/>
-      <c r="R7" s="100"/>
-      <c r="S7" s="109"/>
-      <c r="T7" s="107"/>
-      <c r="U7" s="108"/>
-      <c r="V7" s="99"/>
-      <c r="W7" s="99"/>
-      <c r="X7" s="100"/>
-      <c r="Y7" s="111"/>
-      <c r="Z7" s="99"/>
-      <c r="AA7" s="99"/>
-      <c r="AB7" s="100"/>
-    </row>
-    <row r="8" spans="2:28" x14ac:dyDescent="0.2">
+      <c r="K7" s="123"/>
+      <c r="N7" s="109"/>
+      <c r="O7" s="110"/>
+      <c r="P7" s="95"/>
+      <c r="Q7" s="95"/>
+      <c r="R7" s="94"/>
+      <c r="S7" s="115"/>
+      <c r="T7" s="113"/>
+      <c r="U7" s="114"/>
+      <c r="V7" s="95"/>
+      <c r="W7" s="95"/>
+      <c r="X7" s="94"/>
+      <c r="Y7" s="101"/>
+      <c r="Z7" s="95"/>
+      <c r="AA7" s="95"/>
+      <c r="AB7" s="94"/>
+    </row>
+    <row r="8" spans="2:28">
       <c r="B8" s="8">
         <f t="shared" ref="B8:B9" si="0">B7+1</f>
         <v>3</v>
       </c>
-      <c r="C8" s="91"/>
+      <c r="C8" s="103"/>
       <c r="D8" s="24" t="s">
-        <v>60</v>
+        <v>129</v>
       </c>
       <c r="E8" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="F8" s="10" t="s">
-        <v>92</v>
-      </c>
-      <c r="G8" s="115">
-        <v>25328</v>
-      </c>
-      <c r="H8" s="115">
-        <v>45389</v>
-      </c>
-      <c r="I8" s="10">
+      <c r="F8" s="120" t="s">
+        <v>132</v>
+      </c>
+      <c r="G8" s="121">
+        <v>25132</v>
+      </c>
+      <c r="H8" s="121">
+        <v>44844</v>
+      </c>
+      <c r="I8" s="120">
         <v>5</v>
       </c>
-      <c r="J8" s="59" t="s">
-        <v>93</v>
-      </c>
-      <c r="K8" s="60"/>
+      <c r="J8" s="122" t="s">
+        <v>90</v>
+      </c>
+      <c r="K8" s="123"/>
       <c r="N8" s="34" t="s">
         <v>57</v>
       </c>
       <c r="O8" s="30">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="P8" s="32">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="Q8" s="32">
-        <v>3</v>
-      </c>
-      <c r="R8" s="33"/>
-      <c r="S8" s="38"/>
-      <c r="T8" s="95" t="s">
-        <v>72</v>
-      </c>
-      <c r="U8" s="96"/>
+        <v>1</v>
+      </c>
+      <c r="R8" s="33">
+        <v>1</v>
+      </c>
+      <c r="S8" s="38">
+        <v>1</v>
+      </c>
+      <c r="T8" s="107" t="s">
+        <v>136</v>
+      </c>
+      <c r="U8" s="108"/>
       <c r="V8" s="2">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="W8" s="32">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="X8" s="33">
         <v>0</v>
       </c>
       <c r="Y8" s="37" t="s">
-        <v>72</v>
+        <v>137</v>
       </c>
       <c r="Z8" s="2">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="AA8" s="32">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="AB8" s="33">
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="2:28" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:28">
       <c r="B9" s="8">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="C9" s="91"/>
+      <c r="C9" s="103"/>
       <c r="D9" s="24" t="s">
-        <v>126</v>
+        <v>131</v>
       </c>
       <c r="E9" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="F9" s="10" t="s">
-        <v>94</v>
-      </c>
-      <c r="G9" s="115">
+      <c r="F9" s="120" t="s">
+        <v>91</v>
+      </c>
+      <c r="G9" s="121">
         <v>45385</v>
       </c>
-      <c r="H9" s="115">
+      <c r="H9" s="121">
         <v>17418</v>
       </c>
-      <c r="I9" s="10">
+      <c r="I9" s="120">
         <v>4</v>
       </c>
-      <c r="J9" s="59" t="s">
-        <v>95</v>
-      </c>
-      <c r="K9" s="60"/>
-    </row>
-    <row r="10" spans="2:28" x14ac:dyDescent="0.2">
+      <c r="J9" s="122" t="s">
+        <v>92</v>
+      </c>
+      <c r="K9" s="123"/>
+    </row>
+    <row r="10" spans="2:28">
       <c r="B10" s="8">
         <f>B9+1</f>
         <v>5</v>
       </c>
-      <c r="C10" s="91"/>
+      <c r="C10" s="103"/>
       <c r="D10" s="24" t="s">
-        <v>60</v>
-      </c>
-      <c r="F10" s="6" t="s">
-        <v>98</v>
-      </c>
-      <c r="G10" s="116">
+        <v>59</v>
+      </c>
+      <c r="F10" s="120" t="s">
+        <v>133</v>
+      </c>
+      <c r="G10" s="121">
         <v>45385</v>
       </c>
-      <c r="H10" s="116">
+      <c r="H10" s="121">
         <v>45389</v>
       </c>
-      <c r="I10" s="6">
+      <c r="I10" s="120">
         <v>-2</v>
       </c>
-      <c r="J10" s="61" t="s">
-        <v>99</v>
-      </c>
-      <c r="K10" s="62"/>
-    </row>
-    <row r="11" spans="2:28" x14ac:dyDescent="0.2">
+      <c r="J10" s="122" t="s">
+        <v>96</v>
+      </c>
+      <c r="K10" s="123"/>
+    </row>
+    <row r="11" spans="2:28">
       <c r="B11" s="8">
         <v>6</v>
       </c>
-      <c r="C11" s="91"/>
+      <c r="C11" s="103"/>
       <c r="D11" s="24"/>
       <c r="E11" s="8" t="s">
-        <v>127</v>
-      </c>
-      <c r="F11" s="26" t="s">
-        <v>107</v>
-      </c>
-      <c r="G11" s="117">
-        <v>25601</v>
-      </c>
-      <c r="H11" s="117">
-        <v>25602</v>
-      </c>
-      <c r="I11" s="26">
-        <v>3</v>
-      </c>
-      <c r="J11" s="83" t="s">
+        <v>134</v>
+      </c>
+      <c r="F11" s="120" t="s">
+        <v>132</v>
+      </c>
+      <c r="G11" s="121">
+        <v>37915</v>
+      </c>
+      <c r="H11" s="121">
+        <v>44844</v>
+      </c>
+      <c r="I11" s="120">
+        <v>1</v>
+      </c>
+      <c r="J11" s="122" t="s">
         <v>36</v>
       </c>
-      <c r="K11" s="84"/>
-    </row>
-    <row r="12" spans="2:28" x14ac:dyDescent="0.2">
+      <c r="K11" s="123"/>
+    </row>
+    <row r="12" spans="2:28">
       <c r="B12" s="8">
         <v>7</v>
       </c>
-      <c r="C12" s="91"/>
+      <c r="C12" s="103"/>
       <c r="D12" s="24"/>
       <c r="E12" s="8" t="s">
-        <v>128</v>
-      </c>
-      <c r="F12" s="17" t="s">
-        <v>116</v>
-      </c>
-      <c r="G12" s="118">
+        <v>123</v>
+      </c>
+      <c r="F12" s="124" t="s">
+        <v>113</v>
+      </c>
+      <c r="G12" s="121">
         <v>25601</v>
       </c>
-      <c r="H12" s="118">
+      <c r="H12" s="121">
         <v>25602</v>
       </c>
-      <c r="I12" s="13" t="s">
-        <v>117</v>
-      </c>
-      <c r="J12" s="61" t="s">
+      <c r="I12" s="120" t="s">
+        <v>114</v>
+      </c>
+      <c r="J12" s="122" t="s">
         <v>36</v>
       </c>
-      <c r="K12" s="62"/>
-    </row>
-    <row r="13" spans="2:28" x14ac:dyDescent="0.2">
+      <c r="K12" s="123"/>
+    </row>
+    <row r="13" spans="2:28">
       <c r="B13" s="8">
         <v>8</v>
       </c>
-      <c r="C13" s="91"/>
+      <c r="C13" s="103"/>
       <c r="D13" s="24"/>
       <c r="E13" s="8" t="s">
-        <v>129</v>
-      </c>
-      <c r="F13" s="25" t="s">
-        <v>118</v>
-      </c>
-      <c r="G13" s="117">
-        <v>25601</v>
-      </c>
-      <c r="H13" s="117">
-        <v>25602</v>
-      </c>
-      <c r="I13" s="26">
+        <v>135</v>
+      </c>
+      <c r="F13" s="120" t="s">
+        <v>132</v>
+      </c>
+      <c r="G13" s="121">
+        <v>37915</v>
+      </c>
+      <c r="H13" s="121">
+        <v>44844</v>
+      </c>
+      <c r="I13" s="120">
         <v>0</v>
       </c>
-      <c r="J13" s="83" t="s">
-        <v>99</v>
-      </c>
-      <c r="K13" s="84"/>
-    </row>
-    <row r="14" spans="2:28" x14ac:dyDescent="0.2">
+      <c r="J13" s="122" t="s">
+        <v>96</v>
+      </c>
+      <c r="K13" s="123"/>
+    </row>
+    <row r="14" spans="2:28">
       <c r="B14" s="8">
         <v>9</v>
       </c>
-      <c r="C14" s="91"/>
+      <c r="C14" s="103"/>
       <c r="D14" s="24"/>
       <c r="E14" s="8" t="s">
-        <v>131</v>
-      </c>
-      <c r="F14" s="25" t="s">
-        <v>119</v>
-      </c>
-      <c r="G14" s="117">
+        <v>125</v>
+      </c>
+      <c r="F14" s="124" t="s">
+        <v>116</v>
+      </c>
+      <c r="G14" s="121">
         <v>25601</v>
       </c>
-      <c r="H14" s="117">
+      <c r="H14" s="121">
         <v>25602</v>
       </c>
-      <c r="I14" s="26">
+      <c r="I14" s="120">
         <v>-1</v>
       </c>
-      <c r="J14" s="83" t="s">
-        <v>99</v>
-      </c>
-      <c r="K14" s="84"/>
-    </row>
-    <row r="15" spans="2:28" x14ac:dyDescent="0.2">
+      <c r="J14" s="122" t="s">
+        <v>96</v>
+      </c>
+      <c r="K14" s="123"/>
+    </row>
+    <row r="15" spans="2:28">
       <c r="B15" s="8">
         <v>10</v>
       </c>
-      <c r="C15" s="91"/>
+      <c r="C15" s="103"/>
       <c r="D15" s="24"/>
       <c r="E15" s="8" t="s">
-        <v>130</v>
-      </c>
-      <c r="F15" s="25" t="s">
-        <v>120</v>
-      </c>
-      <c r="G15" s="117">
+        <v>124</v>
+      </c>
+      <c r="F15" s="124" t="s">
+        <v>117</v>
+      </c>
+      <c r="G15" s="121">
         <v>25569</v>
       </c>
-      <c r="H15" s="26" t="s">
-        <v>121</v>
-      </c>
-      <c r="I15" s="26">
+      <c r="H15" s="120" t="s">
+        <v>118</v>
+      </c>
+      <c r="I15" s="120">
         <v>2</v>
       </c>
-      <c r="J15" s="83" t="s">
+      <c r="J15" s="122" t="s">
         <v>36</v>
       </c>
-      <c r="K15" s="84"/>
-    </row>
-    <row r="16" spans="2:28" x14ac:dyDescent="0.2">
+      <c r="K15" s="123"/>
+    </row>
+    <row r="16" spans="2:28">
       <c r="B16" s="8">
         <v>11</v>
       </c>
-      <c r="C16" s="91"/>
+      <c r="C16" s="103"/>
       <c r="D16" s="24"/>
-      <c r="E16" s="119" t="s">
-        <v>132</v>
-      </c>
-      <c r="F16" s="17" t="s">
-        <v>122</v>
-      </c>
-      <c r="G16" s="118">
+      <c r="E16" s="51" t="s">
+        <v>126</v>
+      </c>
+      <c r="F16" s="124" t="s">
+        <v>119</v>
+      </c>
+      <c r="G16" s="121">
         <v>25568</v>
       </c>
-      <c r="H16" s="118">
+      <c r="H16" s="121">
         <v>25602</v>
       </c>
-      <c r="I16" s="13">
+      <c r="I16" s="120">
         <v>4</v>
       </c>
-      <c r="J16" s="61" t="s">
-        <v>123</v>
-      </c>
-      <c r="K16" s="62"/>
-    </row>
-    <row r="17" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="J16" s="122" t="s">
+        <v>120</v>
+      </c>
+      <c r="K16" s="123"/>
+    </row>
+    <row r="17" spans="2:11">
       <c r="B17" s="8">
         <v>12</v>
       </c>
-      <c r="C17" s="91"/>
+      <c r="C17" s="103"/>
       <c r="D17" s="24"/>
       <c r="E17" s="8" t="s">
-        <v>133</v>
-      </c>
-      <c r="F17" s="26" t="s">
-        <v>124</v>
-      </c>
-      <c r="G17" s="117">
+        <v>127</v>
+      </c>
+      <c r="F17" s="120" t="s">
+        <v>121</v>
+      </c>
+      <c r="G17" s="121">
         <v>25935</v>
       </c>
-      <c r="H17" s="117">
+      <c r="H17" s="121">
         <v>25602</v>
       </c>
-      <c r="I17" s="26">
+      <c r="I17" s="120">
         <v>8</v>
       </c>
-      <c r="J17" s="83" t="s">
+      <c r="J17" s="122" t="s">
         <v>36</v>
       </c>
-      <c r="K17" s="84"/>
-    </row>
-    <row r="18" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="K17" s="123"/>
+    </row>
+    <row r="18" spans="2:11">
       <c r="B18" s="8">
         <v>13</v>
       </c>
-      <c r="C18" s="91"/>
+      <c r="C18" s="103"/>
       <c r="D18" s="24"/>
       <c r="E18" s="8" t="s">
-        <v>134</v>
-      </c>
-      <c r="F18" s="26" t="s">
-        <v>125</v>
-      </c>
-      <c r="G18" s="117">
+        <v>128</v>
+      </c>
+      <c r="F18" s="120" t="s">
+        <v>122</v>
+      </c>
+      <c r="G18" s="121">
         <v>25202</v>
       </c>
-      <c r="H18" s="117">
+      <c r="H18" s="121">
         <v>25602</v>
       </c>
-      <c r="I18" s="26">
+      <c r="I18" s="120">
         <v>99</v>
       </c>
-      <c r="J18" s="83" t="s">
-        <v>123</v>
-      </c>
-      <c r="K18" s="84"/>
-    </row>
-    <row r="19" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="J18" s="122" t="s">
+        <v>120</v>
+      </c>
+      <c r="K18" s="123"/>
+    </row>
+    <row r="19" spans="2:11">
       <c r="B19" s="21"/>
       <c r="C19" s="21"/>
       <c r="D19" s="22"/>
@@ -3975,32 +4048,19 @@
       <c r="J19" s="21"/>
       <c r="K19" s="21"/>
     </row>
-    <row r="20" spans="2:11" ht="14.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="23" spans="2:11" ht="14.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="26" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:11" ht="14.45" customHeight="1"/>
+    <row r="23" spans="2:11" ht="14.45" customHeight="1"/>
+    <row r="26" spans="2:11">
       <c r="J26" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="41">
-    <mergeCell ref="J16:K16"/>
-    <mergeCell ref="J17:K17"/>
-    <mergeCell ref="J18:K18"/>
-    <mergeCell ref="J11:K11"/>
-    <mergeCell ref="J12:K12"/>
-    <mergeCell ref="J13:K13"/>
-    <mergeCell ref="J14:K14"/>
-    <mergeCell ref="J15:K15"/>
-    <mergeCell ref="J6:K6"/>
-    <mergeCell ref="J7:K7"/>
-    <mergeCell ref="J8:K8"/>
-    <mergeCell ref="J9:K9"/>
-    <mergeCell ref="J10:K10"/>
-    <mergeCell ref="X6:X7"/>
-    <mergeCell ref="AA6:AA7"/>
-    <mergeCell ref="AB6:AB7"/>
-    <mergeCell ref="Y5:AB5"/>
-    <mergeCell ref="Y6:Y7"/>
-    <mergeCell ref="Z6:Z7"/>
+    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="J4:K4"/>
+    <mergeCell ref="F4:I4"/>
+    <mergeCell ref="E4:E5"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="B3:K3"/>
     <mergeCell ref="W3:X3"/>
     <mergeCell ref="C6:C18"/>
     <mergeCell ref="B4:B5"/>
@@ -4017,35 +4077,34 @@
     <mergeCell ref="T6:U7"/>
     <mergeCell ref="S6:S7"/>
     <mergeCell ref="W6:W7"/>
-    <mergeCell ref="B1:E1"/>
-    <mergeCell ref="J4:K4"/>
-    <mergeCell ref="F4:I4"/>
-    <mergeCell ref="E4:E5"/>
-    <mergeCell ref="C4:C5"/>
-    <mergeCell ref="B3:K3"/>
+    <mergeCell ref="X6:X7"/>
+    <mergeCell ref="AA6:AA7"/>
+    <mergeCell ref="AB6:AB7"/>
+    <mergeCell ref="Y5:AB5"/>
+    <mergeCell ref="Y6:Y7"/>
+    <mergeCell ref="Z6:Z7"/>
+    <mergeCell ref="J6:K6"/>
+    <mergeCell ref="J7:K7"/>
+    <mergeCell ref="J8:K8"/>
+    <mergeCell ref="J9:K9"/>
+    <mergeCell ref="J10:K10"/>
+    <mergeCell ref="J16:K16"/>
+    <mergeCell ref="J17:K17"/>
+    <mergeCell ref="J18:K18"/>
+    <mergeCell ref="J11:K11"/>
+    <mergeCell ref="J12:K12"/>
+    <mergeCell ref="J13:K13"/>
+    <mergeCell ref="J14:K14"/>
+    <mergeCell ref="J15:K15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
+  <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010058284A30843C9F43BD758DDD8294D484" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="6d50638930d08c51b5585735b2be047e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="fed1744a-f275-4023-9290-77fd546fd730" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4acb07121b76573bb3c966f3dcb1b903" ns2:_="">
     <xsd:import namespace="fed1744a-f275-4023-9290-77fd546fd730"/>
@@ -4189,24 +4248,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2BC1EB47-4FFF-47F3-894F-DED91590EA19}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FF0EB622-FDCF-4321-9FF5-C0B282D1670E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{33EFF49E-866D-4BFD-B7FD-9BB436667B53}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4222,4 +4279,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FF0EB622-FDCF-4321-9FF5-C0B282D1670E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2BC1EB47-4FFF-47F3-894F-DED91590EA19}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>